<commit_message>
Updated Latest 18 Aug
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/data.xlsx
+++ b/src/test/resources/testdata/data.xlsx
@@ -39,7 +39,7 @@
   </si>
   <si>
     <t xml:space="preserve">{
-    "name": "morpheus",
+    "name": "morphedus",
     "job": "leader"
 }</t>
   </si>
@@ -238,7 +238,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -264,7 +264,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
has a issue in put request method.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/data.xlsx
+++ b/src/test/resources/testdata/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t xml:space="preserve">RequestURL</t>
   </si>
@@ -54,6 +54,18 @@
     "email": "eve.holt@reqres.in",
     "password": "pistol"
 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/users/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "name": "morpheus",
+    "job": "zion resident"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">put</t>
   </si>
 </sst>
 </file>
@@ -238,7 +250,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:D2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -297,10 +309,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:D2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -340,6 +352,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Enhancement and workable test execution
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/data.xlsx
+++ b/src/test/resources/testdata/data.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="RegisterUserTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="EditUserTest" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t xml:space="preserve">RequestURL</t>
   </si>
@@ -309,10 +310,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -346,26 +347,72 @@
         <v>8</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C2" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>